<commit_message>
Change schema to English
</commit_message>
<xml_diff>
--- a/sample data/Xlsx_sample_data.xlsx
+++ b/sample data/Xlsx_sample_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TuringMac\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TuringMac\Desktop\HITDB-Preprocessing\sample data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,45 +20,13 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Universities" localSheetId="1">Partners!$A$105</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="516">
   <si>
-    <t>序号</t>
-  </si>
-  <si>
-    <t>姓名</t>
-  </si>
-  <si>
-    <t>职务类型</t>
-  </si>
-  <si>
-    <t>教育背景</t>
-  </si>
-  <si>
-    <t>是否是华人</t>
-  </si>
-  <si>
-    <r>
-      <t>所获荣誉或</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Title</t>
-    </r>
-  </si>
-  <si>
-    <t>研究方向</t>
-  </si>
-  <si>
     <t>Trevor Darrell</t>
   </si>
   <si>
@@ -140,136 +108,69 @@
     <t>Graduate Student Researchers</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>有几个博士学生</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DengXian Light"/>
-        <charset val="134"/>
-      </rPr>
-      <t>博士后学生</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DengXian Light"/>
-        <charset val="134"/>
-      </rPr>
-      <t>硕士学生</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/RA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="DengXian Light"/>
-        <charset val="134"/>
-      </rPr>
-      <t>等团队成员</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>UCB EECS, MIT EECS</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>California Department of Transportation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Chair of the State Chapters Council for ITS-America, Ex-Officio member of the Board of Directors to ITS America, member of the Transportation Safety Advancement Group</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Risk Management Solutions, Streamline Solutions, Countrywide Home Loans, IdeaBlade Inc., ezboard, ObjectWare Inc., Texas Instruments</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Driver-assistance systems, vehicular safety systems, highway network safety assessment.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>International Journal of ITS Research, ITS Best of ITS Research Award</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Forensic Technologies International, Automotive Technology International, Breed Automotive Corporation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>ASME DSCD’s Charles Stark Draper Award, American Automatic Control Council’s Control Engineering Practice Award</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Federal  Highway  Administration, Caltrans, Federal Highway Administration, National Automated Highway System Consortium</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Alexander Skabardonis</t>
   </si>
   <si>
     <t>PhD. (University of Southampton)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Traffic flow theory and models, traffic management and control systems, intelligent transportation systems</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Wei-Bin Zhang</t>
   </si>
   <si>
     <t>PhD. (Northern Jiaotong University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Northern Jiaotong University</t>
   </si>
   <si>
     <t>YES</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Railway control systems</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Elaine Banks</t>
@@ -285,85 +186,53 @@
   </si>
   <si>
     <t>Matthew Barth</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>兼职</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>以往雇主</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>UCR</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (UCSB)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Engineering system concepts and automation technology </t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>TRB Pyke Johnson Award, winner of the Connected Vehicle Technology Challenge</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Alexandre Bayen</t>
   </si>
   <si>
     <t>PhD. (Stanford University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Ballhaus Award, NASA Top 10 Innovators, TRANNY Award, Presidential Early Career Award, Okawa Research Grant Award,IEEE  Ruberti Prize, ASCE Huber Prize</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Control theory, optimization, mobile sensing and transportation engineering</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">KarMode, Nokia, BAE Systems, NASA </t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Evelyn Blumenberg</t>
   </si>
   <si>
     <t>Residential location</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (UCLA)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Chair of the Department of Urban Planning</t>
@@ -373,108 +242,76 @@
   </si>
   <si>
     <t>PhD. (ETH-Zurich)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2009 NSF CAREER Award, 2012 IEEE Control System Technology Award</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IEEE fellow</t>
   </si>
   <si>
     <t>BrightBox Technologies Inc, Hyundai Center of Excellence</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Advanced automotive control and energy efficient building operation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>是否是某学术期刊的编辑或学术会议的组委会成员</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>专业委员会</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Transportation Research Part C, Journal of Intelligent Transportation Systems and IET Intelligent Transport Systems, Bus and truck platoon systems, cooperative ACC systems</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Intelligent Transportation Systems Journal, 19th International Symposium on Transportation and Traffic Theory (ISTTT19), Member of Transportation Research Board/National Research Council, Freeway Operations Committee, Highway Capacity and Quality of Service Committee. Traffic Signal Systems Committee, Simulation SubCommittee</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IEEE Fellow, Board of Governor, TRB, ITS America and APTA, senior member of IEEE, Vice President for Conference of IEEE ITS Society</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IEEE Intelligent Transportation System Society, Transactions of ITS, IEEE ITSS Board of Governors, IEEE ITSS President</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>White House Champion of Change</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Mike Cassidy</t>
   </si>
   <si>
     <t>Traffic and transportation operations, Traffic control, Public transit</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (UCB)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Chancellor's Professorship, 2014 Cunard Award for best paper from the Operations Section of the Transportation Research Board</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Transportation Research Part B, Robert Horonjeff Endowed Chair in Civil Engineering</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Tom Durbin</t>
   </si>
   <si>
     <t>Vehicle emissions with on studying fuels, advanced technology vehicles, particle and in-use emissions</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Intergovernmental Panel on Climate Change</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (UCR)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Karl Hedrick</t>
@@ -484,22 +321,22 @@
   </si>
   <si>
     <t>Rufus Oldenburger Medal</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>National Academy of Engineering</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Roberto Horowitz</t>
   </si>
   <si>
     <t>Applications to traffic modeling, estimation and management, Intelligent Vehicle and Highway Systems</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IBM Young Faculty Development Award, NSF Presidential Young Investigator Award, Japanese Ministry of Education Foreign Researcher Award, 2005 American Automatic Control Council (AACC) Hugo Shuck Best Application Paper Award, 2010 ASME Dynamic Systems and Control Division (DSCD) Henry M. Paynter Outstanding Research Award</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">DSCD </t>
@@ -512,52 +349,52 @@
   </si>
   <si>
     <t>Distinguished Engineering Aluni Award, James Laurie Prize, Fannie and John Herz Foundation Award, Robert Horonjeff Award, Walter L. Huber Civil Engineering Research Prize</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> National Academy of Engineering</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Tim Lipman</t>
   </si>
   <si>
     <t>Electric-drive vehicles, fuel cell technology, combined heat and power systems, biofuels, renewable energy, and electricity and hydrogen energy systems infrastructure</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (UCD)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2005 Climate Change Fellow</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2004 Institute of Transportation Engineers service award, 1997&amp;1995 University of California Transportation Center Dissertation Grant</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Alexey Pozdnukhov</t>
   </si>
   <si>
     <t>PhD. (EPFL)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Machine learning, spatial data mining, computational social science, urban mobility, smart cities</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>David Ragland</t>
   </si>
   <si>
     <t>Injury epidemiology, Injuries in vulnerable roads users, Interaction of behavioral and environmental factors in injury, Demographic/social/cultural factors in injury patterns, Firearm injury</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Governor's Office of Planning and Research, California Department of Public Health, California Strategic Highway Safety Plan (SHSP), California Pedestrian Advisory Committee</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Raja Sengupta</t>
@@ -567,26 +404,26 @@
   </si>
   <si>
     <t>PhD. (University of Michigan)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Berkeley Energy and Climate Lectures Curriculum Innovation Award USDOT Connected Vehicle Technology Award 2011</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>CEE</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Susan Shaheen</t>
   </si>
   <si>
     <t>Carsharing, smart parking management, fuel cell, electric, and plug-in hybrid vehicles and infrastructure, smart growth/development</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Honda Distinguished Scholar in Transportation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -602,7 +439,7 @@
       </rPr>
       <t xml:space="preserve"> chair of the subcommittee for Shared-Use Vehicle Public Transport Systems of TRB</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Executive Associate Dean</t>
@@ -612,7 +449,7 @@
   </si>
   <si>
     <t>Masayoshi Tomizuka</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Pravin Varaiya</t>
@@ -622,39 +459,35 @@
   </si>
   <si>
     <t>Discrete Event Dynamical Systems, Transportation Research---C, Fellow of IEEE, American Academy of Arts and Science, member of the National Academy of Engineering</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>UCLA</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Transportation systems, use of performance measurement in transportation planning</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Control, Intelligent Systems, and Robotics, Communications &amp; Networking</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Guggenheim Fellowship, Rockefeller Foundation Humanities Fellowships, UCLA Alumni Association Distinguished Teaching Award, Pyke Johnson Award for the best paper presented at an annual meeting of the Transportation Research Board (TRB), the Carey Award for service to the TRB.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (Northwestern University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Joan Walker</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Martin Wachs</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>E-mail</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>trevor@eecs.berkeley.edu</t>
@@ -739,37 +572,37 @@
   </si>
   <si>
     <t>joanwalker@berkeley.edu</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Discrete choice analysis and travel behavior</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Boston University</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Presidential Early Career Award</t>
   </si>
   <si>
     <t>Transportation Science, Chair of the Committee on Transportation Demand Forecasting (ADB40) for the Transportation Research Board of the National Academies</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Qijian Gan</t>
   </si>
   <si>
     <t>UCI</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (University of California, Irvine)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Network traffic flow theory, network modeling and simulation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>qgan@uci.edu</t>
@@ -782,7 +615,7 @@
   </si>
   <si>
     <t>PhD. (Tianjin University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -807,11 +640,11 @@
       </rPr>
       <t xml:space="preserve"> Nanyang Technological University, Singapore, Beijing Jiaotong University</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Wireless sensor networks, vehicular networking, and next-generation Internet</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>gdeyun@gmail.com</t>
@@ -821,22 +654,22 @@
   </si>
   <si>
     <t>PhD. (National Taiwan University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>National Chiao Tung University</t>
   </si>
   <si>
     <t>Mobile computing, wireless networks, data mining and cloud computing</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Chair of BigPMA</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IEEE CIG 2015, ICPP 2011, TAAI 2010, MDM 2010, ACM Transactions on Sensor Networks, VLDB Journal, IEEE Transactions on Knowledge and Data Engineering, IEEE Transactions on Mobile Computing…</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>jlhuang@cs.nctu.edu.tw</t>
@@ -852,29 +685,29 @@
   </si>
   <si>
     <t xml:space="preserve">Toshiba, Sandex, </t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>M.S. (Tokyo University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Qingzhou Mao</t>
   </si>
   <si>
     <t>qzhmao@whu.edu.cn</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Wuhan University</t>
   </si>
   <si>
     <t>Satellite navigation system, remote sensing and geographic information system integration, high-precision laser measurement, pattern recognition and vision measurement technology</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (Wuhan University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cédric Mauquoi</t>
@@ -884,15 +717,15 @@
   </si>
   <si>
     <t>M.S. (ETHZ)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Robotic behaviour, use of machine learning in Computer Vision</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Soltar AG, Contexa</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Paul Mustière</t>
@@ -902,15 +735,15 @@
   </si>
   <si>
     <t>M.S. (MINES ParisTech)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Machine learning and AI</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Fluent.ai, Université Pierre et Marie Curie, Groupe Ponticelli Frères</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Hua Qin</t>
@@ -929,11 +762,11 @@
   </si>
   <si>
     <t>Systems modelling, simulation, control systems design and multi-sensor data fusion</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (Tsinghua University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Dali Wei</t>
@@ -943,7 +776,7 @@
   </si>
   <si>
     <t>PhD. (Texas Tech University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Intelligent Transportation Systems, Traffic Simulation, and Traffic Signal Control and Optimization</t>
@@ -956,15 +789,15 @@
   </si>
   <si>
     <t>Caltrans, UMTRI, VTTI</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PhD. (University of Waterloo)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Traffic Engineering, Traffic simulation modeling, Driver Behavior modeling, Vehicle emission modeling</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Gary Gremaux</t>
@@ -974,11 +807,11 @@
   </si>
   <si>
     <t>Data analysis and database management and programming</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>M.S. (UCI)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Lisa Hammon</t>
@@ -988,45 +821,45 @@
   </si>
   <si>
     <t>Transportation Project Management, Grant Writing for Transportation Projects and Programs, City and Regional Government Administration</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>City of Hercules, CA, Marina Village, North Star Computers</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>B.S. (UCB)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Michelle Harrington</t>
   </si>
   <si>
     <t>Overseeing the Connected Corridors quarterly newsletter, updating the project's website and providing other communication items</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>B.S. (California State University, East Bay)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Tom Kuhn</t>
   </si>
   <si>
     <t>WCCTAC</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Architecture and implementation of software</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>M.S. (Stanford University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Nuance Communications, CombineNet Inc.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>tmk@path.berkeley.edu</t>
@@ -1039,15 +872,15 @@
   </si>
   <si>
     <t>Software development, systems design and systems integration</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>UCSD, Lilly Singapore Centre for Drug Discovery, Sequenom, Accredited Home Lenders, SciTegic, Inc, Accelrys, National Center for Genome Resources, Logicon, Inc</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>M.S. (Bowling Green State University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Benjamin McKeever</t>
@@ -1057,15 +890,15 @@
   </si>
   <si>
     <t>Development and growth of a robust and coherent program</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Operations R&amp;D</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>M.S. (University of Texas at Austin)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Greg Merritt</t>
@@ -1075,11 +908,11 @@
   </si>
   <si>
     <t>Data acquisition, analysis, and visualization, providing systems and network engineering support, machine learning and sentiment analysis</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>M.S. (University of Michigan, Ann Arbor)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Sean Morris</t>
@@ -1089,7 +922,7 @@
   </si>
   <si>
     <t>Web mapping and javascript programming technologies and techniques</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Albany High School in Albany</t>
@@ -1108,15 +941,15 @@
   </si>
   <si>
     <t>Systems Engineering, Systems Architecture, Application Development, Project &amp; Program Management</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>B.S. (Iowa State University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>U.S. Navy, the U.S. Air Force’s Wright Research and Development Center, ARINC</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>John Spring</t>
@@ -1126,11 +959,11 @@
   </si>
   <si>
     <t>Software systems for the command and control of vehicles and infrastructure</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>M.S. (San Francisco State University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Nathaniel Titterton</t>
@@ -1140,7 +973,7 @@
   </si>
   <si>
     <t>User-interface, visualization, reporting, and related systems</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Fred Winik</t>
@@ -1150,15 +983,11 @@
   </si>
   <si>
     <t>Developeing documentation and web content on hybrid data, Integrated Corridor Management (ICM), and systems engineering</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>M.S. (UCB)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>近三年学术文章数量</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Gabriel Gomes</t>
@@ -1168,11 +997,11 @@
   </si>
   <si>
     <t>Traffic modeling, simulation, control</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>CCIT</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Julien Jacquemot</t>
@@ -1182,11 +1011,11 @@
   </si>
   <si>
     <t>M.S. (Ecole Polytechnique, Ecole Polytechnique Federale of Lausanne)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Alzheimer’s disease, machine learning, computer vision and mobile sensing</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Alexander A. Kurzhanskiy</t>
@@ -1196,7 +1025,7 @@
   </si>
   <si>
     <t>Transportation, Dynamical Systems, Cyber-Physical Systems, Information Technology</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Xiao-Yun Lu</t>
@@ -1206,14 +1035,14 @@
   </si>
   <si>
     <t>PhD. (University of Manchester)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">University of Leicester UK </t>
   </si>
   <si>
     <t>Traffic systems detection, modeling, control design, micro/macro simulation, real-time implementation, vehicle system modeling and longitudinal control</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Michael Mauch</t>
@@ -1223,33 +1052,33 @@
   </si>
   <si>
     <t>Transportation data analysis, applications programming, mathematical model building, travel demand forecasting</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Sacramento State Universit, UCD</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Huadong (Joshua) Meng</t>
   </si>
   <si>
     <t>hdmeng@berkeley.edu</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Statistical signal processing, intelligent transportation systems, remote sensing and localization</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Tsinghua University</t>
   </si>
   <si>
     <t>Tsinghua University</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>IEEE Transactions on SP/IP/AES, IET Signal Processing, IET RSN, Chinese Journal of Electronics</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Anthony Patire</t>
@@ -1259,7 +1088,7 @@
   </si>
   <si>
     <t>GPS-based probe data, data assimilation, flow models, integrated corridor management</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Kun Zhou</t>
@@ -1275,7 +1104,7 @@
   </si>
   <si>
     <t>Transit schedules</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Jane Street</t>
@@ -1291,7 +1120,7 @@
   </si>
   <si>
     <t>Policy research, employee reimbursements, creating weekly reports</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Zahra Amini</t>
@@ -1301,7 +1130,7 @@
   </si>
   <si>
     <t>Traffic and transportation operation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Fang-Chieh Chou</t>
@@ -1311,11 +1140,11 @@
   </si>
   <si>
     <t>M.S. (National Taiwan University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>V2X communications for automated vehicles</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Marco Innao</t>
@@ -1325,15 +1154,15 @@
   </si>
   <si>
     <t>M.S. (University of Bologna, UCB)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Developing optimization models for coordinated freeway ramp metering and traffic signals</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Inter-American Development Bank, Savino Del Bene, EMBARQ</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>David Kan</t>
@@ -1343,7 +1172,7 @@
   </si>
   <si>
     <t>Coordination of Freeway Ramp Metering and Arterial Traffic Signals</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>San Francisco Municipal Transportation Agency (SFMTA)</t>
@@ -1356,7 +1185,7 @@
   </si>
   <si>
     <t>Congestion-Responsive On-Ramp Metering</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Negar Zahedi Mehr</t>
@@ -1366,11 +1195,11 @@
   </si>
   <si>
     <t>B.S. (Sharif University of Technology)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Applications in traffic control and transportation engineering</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Brian Phegley</t>
@@ -1380,26 +1209,26 @@
   </si>
   <si>
     <t>Fault Detection of Freeway Loop Detectors</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Matthew Wright</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>mwright@berkeley.edu</t>
   </si>
   <si>
     <t>Simulation, statistical analysis, control strategies for large-scale dynamical systems</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>HERE</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>B.S. (University of Texas at Austin)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Virginia and Ernest Cockrell, Jr. Scholarship in Engineering</t>
@@ -1412,11 +1241,11 @@
   </si>
   <si>
     <t>M.S. (MIT)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Intersection of control theory, optimization, statistics, cyber-physical systems</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cheng-Ju Wu</t>
@@ -1426,11 +1255,11 @@
   </si>
   <si>
     <t>Freeway traffic demand prediction, Freeway traffic modeling and control strategies simulation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>B.S. (National Taiwan University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Yiqing Yao</t>
@@ -1440,11 +1269,11 @@
   </si>
   <si>
     <t>B.S. (Southeast University)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Vehicle automation and vehicular cooperative positioning</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Wei Zhan</t>
@@ -1454,14 +1283,14 @@
   </si>
   <si>
     <t>M.S. (Harbin Institute of Technology)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>University of Hong Kong</t>
   </si>
   <si>
     <t>Urban autonomous driving</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>California Department of Transportation (Caltrans)</t>
@@ -1732,7 +1561,7 @@
   </si>
   <si>
     <t>AC Transit (Alameda-Contra Costa Transit District)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Alaska Department of Transportation</t>
@@ -1910,13 +1739,49 @@
   </si>
   <si>
     <t>Utah State University</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Awards</t>
+  </si>
+  <si>
+    <t>Fellow</t>
+  </si>
+  <si>
+    <t>Research area</t>
+  </si>
+  <si>
+    <t>Students</t>
+  </si>
+  <si>
+    <t>Papers</t>
+  </si>
+  <si>
+    <t>Past-employer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1929,12 +1794,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="DengXian Light"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2007,7 +1866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -2045,7 +1904,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2355,7 +2214,7 @@
   <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2375,42 +2234,42 @@
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="16" customFormat="1" ht="58.5">
+    <row r="1" spans="1:12" s="16" customFormat="1" ht="31.5">
       <c r="A1" s="16" t="s">
-        <v>0</v>
+        <v>505</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>1</v>
+        <v>506</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>2</v>
+        <v>507</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>3</v>
+        <v>508</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>4</v>
+        <v>509</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>5</v>
+        <v>510</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>77</v>
+        <v>511</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>6</v>
+        <v>512</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>34</v>
+        <v>513</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>278</v>
+        <v>514</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>57</v>
+        <v>515</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>137</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2418,21 +2277,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="I2" s="6">
         <v>14</v>
@@ -2441,10 +2300,10 @@
         <v>31</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2452,24 +2311,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2477,28 +2336,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I4" s="6"/>
       <c r="K4" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2506,35 +2365,35 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="1">
         <v>33</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2542,31 +2401,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2574,28 +2433,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="J7" s="1">
         <v>12</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2603,28 +2462,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2632,16 +2491,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2649,17 +2508,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2667,16 +2526,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2684,16 +2543,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2701,31 +2560,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2733,31 +2592,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="J14" s="1">
         <v>10</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2765,31 +2624,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="J15" s="1">
         <v>2</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2797,25 +2656,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I16" s="1">
         <v>18</v>
@@ -2824,10 +2683,10 @@
         <v>37</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -2835,25 +2694,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I17" s="1">
         <v>4</v>
@@ -2862,7 +2721,7 @@
         <v>6</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -2870,28 +2729,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -2899,25 +2758,25 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I19" s="1">
         <v>18</v>
@@ -2926,7 +2785,7 @@
         <v>2</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -2934,25 +2793,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="I20" s="1">
         <v>37</v>
@@ -2961,7 +2820,7 @@
         <v>20</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2969,28 +2828,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2998,31 +2857,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="J22" s="1">
         <v>2</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -3030,25 +2889,25 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="J23" s="1">
         <v>6</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -3056,26 +2915,26 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="J24" s="1">
         <v>10</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -3083,31 +2942,31 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J25" s="1">
         <v>6</v>
       </c>
       <c r="L25" s="14" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -3115,28 +2974,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="L26" s="14" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -3144,28 +3003,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="I27" s="1">
         <v>25</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -3173,31 +3032,31 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="I28" s="1">
         <v>2</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -3205,28 +3064,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="L29" s="14" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -3234,25 +3093,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="I30" s="1">
         <v>9</v>
@@ -3261,10 +3120,10 @@
         <v>11</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="L30" s="14" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -3272,31 +3131,31 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J31" s="1">
         <v>5</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="L31" s="14" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -3304,28 +3163,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="J32" s="1">
         <v>6</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="L32" s="14" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -3333,34 +3192,34 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="J33" s="1">
         <v>12</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="L33" s="14" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -3368,25 +3227,25 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="L34" s="14" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -3394,28 +3253,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="J35" s="1">
         <v>8</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="L35" s="14" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -3423,25 +3282,25 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="L36" s="14" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -3449,25 +3308,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="L37" s="14" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -3475,25 +3334,25 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="J38" s="1">
         <v>5</v>
       </c>
       <c r="L38" s="14" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -3501,25 +3360,25 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="J39" s="1">
         <v>3</v>
       </c>
       <c r="L39" s="14" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -3527,25 +3386,25 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="J40" s="1">
         <v>3</v>
       </c>
       <c r="L40" s="14" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -3553,25 +3412,25 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="L41" s="14" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -3579,22 +3438,22 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -3602,28 +3461,28 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="L43" s="14" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -3631,19 +3490,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -3651,25 +3510,25 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="L45" s="14" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -3677,25 +3536,25 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="L46" s="14" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -3703,25 +3562,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="L47" s="14" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -3729,22 +3588,22 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="L48" s="14" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -3752,22 +3611,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="L49" s="14" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -3775,16 +3634,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L50" s="14" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3792,25 +3651,25 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="L51" s="14" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -3818,22 +3677,22 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="L52" s="14" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -3841,22 +3700,22 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="L53" s="14" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -3864,22 +3723,22 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -3887,28 +3746,28 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="J55" s="1">
         <v>3</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="L55" s="14" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -3916,22 +3775,22 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="L56" s="14" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -3939,25 +3798,25 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="J57" s="1">
         <v>2</v>
       </c>
       <c r="L57" s="14" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -3965,25 +3824,25 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -3991,28 +3850,28 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="J59" s="1">
         <v>8</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -4020,28 +3879,28 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="L60" s="14" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -4049,22 +3908,22 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="L61" s="14" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -4072,16 +3931,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="L62" s="14" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -4089,26 +3948,26 @@
         <v>62</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="L63" s="14" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -4116,19 +3975,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="L64" s="14" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -4136,22 +3995,22 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="L65" s="14" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -4159,22 +4018,22 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="L66" s="14" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -4182,25 +4041,25 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="L67" s="14" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -4208,25 +4067,25 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="L68" s="14" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -4234,22 +4093,22 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="L69" s="14" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -4257,22 +4116,22 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="L70" s="14" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -4280,22 +4139,22 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="L71" s="14" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -4303,31 +4162,31 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="J72" s="1">
         <v>4</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="L72" s="14" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -4335,25 +4194,25 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="J73" s="1">
         <v>2</v>
       </c>
       <c r="L73" s="14" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -4361,25 +4220,25 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="J74" s="1">
         <v>3</v>
       </c>
       <c r="L74" s="14" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -4387,22 +4246,22 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="L75" s="14" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -4410,29 +4269,29 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="L76" s="14" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L9" r:id="rId1" display="mailto:ebanks@berkeley.edu"/>
     <hyperlink ref="L10" r:id="rId2" display="mailto:bob.meade@berkeley.edu"/>
@@ -4522,7 +4381,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="19" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -4530,262 +4389,262 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="17" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="17" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="17" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="17" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="17" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="17" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="17" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="17" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="17" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="17" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="17" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="17" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="17" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="17" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="17" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="17" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="17" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="17" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="17" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="17" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="17" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="17" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="17" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="17" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="17" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="17" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="17" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="17" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="17" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="17" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="17" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="17" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="17" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="17" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="17" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="17" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="17" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="17" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="17" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="17" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="17" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="17" t="s">
-        <v>481</v>
+        <v>469</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="17" t="s">
-        <v>482</v>
+        <v>470</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="17" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="17" t="s">
-        <v>483</v>
+        <v>471</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="17" t="s">
-        <v>484</v>
+        <v>472</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="17" t="s">
-        <v>485</v>
+        <v>473</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="17" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="17" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="17" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="17" t="s">
-        <v>486</v>
+        <v>474</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="17" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
     </row>
     <row r="55" spans="1:1">
@@ -4793,7 +4652,7 @@
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="19" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
     </row>
     <row r="57" spans="1:1">
@@ -4801,242 +4660,242 @@
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="17" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="17" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="17" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="17" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="17" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="17" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="17" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="17" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="17" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="17" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="17" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="17" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="17" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="17" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="17" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="17" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="17" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="17" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="17" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="17" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="17" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="17" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="17" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="17" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="17" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="17" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="17" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="17" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="17" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="17" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="17" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="17" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="17" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="17" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="17" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="17" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="17" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="17" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="17" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="17" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="17" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="17" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="17" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="17" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="17" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="17" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" s="17" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="17" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
     </row>
     <row r="106" spans="1:1">
@@ -5044,7 +4903,7 @@
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="19" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
     </row>
     <row r="108" spans="1:1">
@@ -5052,241 +4911,241 @@
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="17" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" s="17" t="s">
-        <v>488</v>
+        <v>476</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="17" t="s">
-        <v>489</v>
+        <v>477</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" s="17" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="17" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" s="17" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="17" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" s="17" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="17" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" s="17" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="17" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" s="17" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="17" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" s="17" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="17" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" s="17" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="17" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" s="17" t="s">
-        <v>495</v>
+        <v>483</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="17" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" s="17" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="17" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" s="17" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="17" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" s="17" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="17" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" s="17" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="17" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" s="17" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" s="17" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" s="17" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" s="17" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" s="17" t="s">
-        <v>505</v>
+        <v>493</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="17" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" s="17" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="17" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" s="17" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="17" t="s">
-        <v>510</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="17" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" s="17" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" s="17" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" s="17" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" s="17" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" s="17" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" s="17" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" s="17" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" s="17" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" s="17" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>